<commit_message>
Migrated all projects to .net standard, and add a new WPF project
</commit_message>
<xml_diff>
--- a/Documentation/DBEntities.xlsx
+++ b/Documentation/DBEntities.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523D0848-14CF-494A-847B-74446D490DA2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8014DDB6-2B0C-4BF8-ACB1-069265CE02A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tblFixedDeposit" sheetId="1" r:id="rId1"/>
-    <sheet name="tblBank" sheetId="2" r:id="rId2"/>
-    <sheet name="tblBankBranch" sheetId="3" r:id="rId3"/>
-    <sheet name="tblUser" sheetId="4" r:id="rId4"/>
-    <sheet name="tblTransaction" sheetId="5" r:id="rId5"/>
-    <sheet name="tblMonthlyPlanner" sheetId="6" r:id="rId6"/>
-    <sheet name="tblInsurance" sheetId="7" r:id="rId7"/>
+    <sheet name="tblLogin" sheetId="8" r:id="rId1"/>
+    <sheet name="tblDevice" sheetId="9" r:id="rId2"/>
+    <sheet name="tblUser" sheetId="4" r:id="rId3"/>
+    <sheet name="tblTransaction" sheetId="5" r:id="rId4"/>
+    <sheet name="tblMonthlyPlanner" sheetId="6" r:id="rId5"/>
+    <sheet name="tblBank" sheetId="2" r:id="rId6"/>
+    <sheet name="tblFixedDeposit" sheetId="1" r:id="rId7"/>
+    <sheet name="tblBankBranch" sheetId="3" r:id="rId8"/>
+    <sheet name="tblInsurance" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>FixedDepositID</t>
   </si>
@@ -187,6 +189,36 @@
   </si>
   <si>
     <t>lstGender</t>
+  </si>
+  <si>
+    <t>LoginId</t>
+  </si>
+  <si>
+    <t>PasswordHash</t>
+  </si>
+  <si>
+    <t>IsEmailVerified</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>IsSessionActive</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>DeviceId</t>
+  </si>
+  <si>
+    <t>DeviceType</t>
+  </si>
+  <si>
+    <t>DeviceHash</t>
+  </si>
+  <si>
+    <t>DeviceSessionId</t>
   </si>
 </sst>
 </file>
@@ -506,6 +538,350 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2D3E8B-17CE-4C82-B036-FF68F35C3019}">
+  <dimension ref="B2:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEBB1AA-EC7D-4E26-B1F6-474A60BA1044}">
+  <dimension ref="B2:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68372321-5CEA-4AC8-B272-F879EF86D314}">
+  <dimension ref="D2:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E673295-7AD3-412D-BE9C-4F4E9BE4CFD7}">
+  <dimension ref="D2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H18"/>
   <sheetViews>
@@ -656,41 +1032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D4"/>
   <sheetViews>
@@ -735,226 +1077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:K7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68372321-5CEA-4AC8-B272-F879EF86D314}">
-  <dimension ref="D2:L21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E673295-7AD3-412D-BE9C-4F4E9BE4CFD7}">
-  <dimension ref="D2:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F8F784-7FFF-447A-AE94-8720F369D0EE}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Login Support for existing user added
</commit_message>
<xml_diff>
--- a/Documentation/DBEntities.xlsx
+++ b/Documentation/DBEntities.xlsx
@@ -1,34 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8014DDB6-2B0C-4BF8-ACB1-069265CE02A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA33B1D-3F86-444C-A495-106099DA4B80}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tblLogin" sheetId="8" r:id="rId1"/>
     <sheet name="tblDevice" sheetId="9" r:id="rId2"/>
     <sheet name="tblUser" sheetId="4" r:id="rId3"/>
-    <sheet name="tblTransaction" sheetId="5" r:id="rId4"/>
-    <sheet name="tblMonthlyPlanner" sheetId="6" r:id="rId5"/>
+    <sheet name="tblMonthlyPlanner" sheetId="6" r:id="rId4"/>
+    <sheet name="tblTransaction" sheetId="5" r:id="rId5"/>
     <sheet name="tblBank" sheetId="2" r:id="rId6"/>
     <sheet name="tblFixedDeposit" sheetId="1" r:id="rId7"/>
     <sheet name="tblBankBranch" sheetId="3" r:id="rId8"/>
     <sheet name="tblInsurance" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>FixedDepositID</t>
   </si>
@@ -219,6 +224,9 @@
   </si>
   <si>
     <t>DeviceSessionId</t>
+  </si>
+  <si>
+    <t>UserId</t>
   </si>
 </sst>
 </file>
@@ -234,12 +242,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,11 +268,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEBB1AA-EC7D-4E26-B1F6-474A60BA1044}">
   <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -686,11 +701,61 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E673295-7AD3-412D-BE9C-4F4E9BE4CFD7}">
+  <dimension ref="D2:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68372321-5CEA-4AC8-B272-F879EF86D314}">
   <dimension ref="D2:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,9 +798,10 @@
       </c>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="E5" s="2"/>
       <c r="L5" t="s">
         <v>48</v>
       </c>
@@ -801,45 +867,6 @@
     <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E673295-7AD3-412D-BE9C-4F4E9BE4CFD7}">
-  <dimension ref="D2:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>